<commit_message>
modification du journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Année 4\Pré TPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreTPI\PreTPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -133,10 +133,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -146,13 +146,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -161,14 +161,14 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
@@ -178,7 +178,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -512,7 +512,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="9">
-        <v>9.375E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>6</v>
@@ -703,7 +703,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +733,10 @@
       <c r="A3" s="6">
         <v>44963</v>
       </c>
+      <c r="B3" s="5">
+        <f>SUM(Journal!C6:C9)</f>
+        <v>0.19791666666666666</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
@@ -740,7 +744,7 @@
       </c>
       <c r="B5" s="5">
         <f>SUM(B2:B4)</f>
-        <v>6.9444444444444434E-2</v>
+        <v>0.2673611111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification de la planification initiale du projet
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Jour</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Nb Heures</t>
+  </si>
+  <si>
+    <t>Modification de la planification initiale du projet, suite au retour du chef de projet</t>
   </si>
 </sst>
 </file>
@@ -164,11 +167,11 @@
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
@@ -237,8 +240,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B5" totalsRowCount="1">
   <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>SUM(B2:B4)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -511,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +524,7 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -678,10 +681,19 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="7">
+        <v>44964</v>
+      </c>
+      <c r="B10" s="8">
+        <v>2</v>
+      </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -702,7 +714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajout de la planification initiale dans le rapport de projet
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Jour</t>
   </si>
@@ -167,11 +167,11 @@
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="21" formatCode="dd/mmm"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="21" formatCode="dd/mmm"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
@@ -223,8 +223,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E12"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="7"/>
     <tableColumn id="2" name="Semaine" dataDxfId="6"/>
@@ -240,8 +240,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B5" totalsRowCount="1">
   <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
       <totalsRowFormula>SUM(B2:B4)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -512,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +687,9 @@
       <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9">
+        <v>4.5138888888888888E-2</v>
+      </c>
       <c r="D10" s="8" t="s">
         <v>6</v>
       </c>
@@ -696,10 +698,27 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="7">
+        <v>44964</v>
+      </c>
+      <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -714,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,13 +769,22 @@
         <v>0.19791666666666666</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>44964</v>
+      </c>
+      <c r="B4" s="5">
+        <f>SUM(Journal!C10:C11)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="5">
         <f>SUM(B2:B4)</f>
-        <v>0.2673611111111111</v>
+        <v>0.3298611111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update rapport de projet
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Jour</t>
   </si>
@@ -223,8 +223,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E13" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E13"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="7"/>
     <tableColumn id="2" name="Semaine" dataDxfId="6"/>
@@ -237,12 +237,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B5" totalsRowCount="1">
-  <autoFilter ref="A1:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B6" totalsRowCount="1">
+  <autoFilter ref="A1:B5"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B4)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B5)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -512,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,10 +715,27 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="7">
+        <v>44966</v>
+      </c>
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -731,10 +748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,12 +796,20 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6">
+        <v>44965</v>
+      </c>
+      <c r="B5" s="5">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
-        <f>SUM(B2:B4)</f>
-        <v>0.3298611111111111</v>
+      <c r="B6" s="5">
+        <f>SUM(B2:B5)</f>
+        <v>0.3923611111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Export des categories sur GLPI
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Jour</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>Modification de la planification initiale du projet, suite au retour du chef de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse de la partie "gestion du parc" sur la nouvelle version de l'application </t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>Export des données des catégories sur l'ancienne version de l'application</t>
   </si>
 </sst>
 </file>
@@ -223,8 +232,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E13" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E14" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E14"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="7"/>
     <tableColumn id="2" name="Semaine" dataDxfId="6"/>
@@ -237,12 +246,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B6" totalsRowCount="1">
-  <autoFilter ref="A1:B5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B7" totalsRowCount="1">
+  <autoFilter ref="A1:B6"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B5)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B6)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,10 +741,38 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8"/>
+      <c r="A13" s="7">
+        <v>44967</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>44967</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -748,10 +785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,19 +834,28 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>44965</v>
+        <v>44966</v>
       </c>
       <c r="B5" s="5">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6">
+        <v>44967</v>
+      </c>
+      <c r="B6" s="5">
+        <f>SUM(Journal!C13:C14)</f>
+        <v>0.10069444444444443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5">
-        <f>SUM(B2:B5)</f>
-        <v>0.3923611111111111</v>
+      <c r="B7" s="5">
+        <f>SUM(B2:B6)</f>
+        <v>0.49305555555555552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des risques techniques sur le rapport
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Jour</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Analyse des templates dans la partie "gestion du parc"</t>
+  </si>
+  <si>
+    <t>Analyse des fermetures de ticket dans la partie "gestion des tckets"</t>
+  </si>
+  <si>
+    <t>Rédaction des problèmes techniques dans le rapport de projet</t>
   </si>
 </sst>
 </file>
@@ -244,8 +250,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E21"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="7"/>
     <tableColumn id="2" name="Semaine" dataDxfId="6"/>
@@ -258,12 +264,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B8" totalsRowCount="1">
-  <autoFilter ref="A1:B7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B9" totalsRowCount="1">
+  <autoFilter ref="A1:B8"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B7)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B8)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,6 +877,40 @@
         <v>25</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>44978</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3</v>
+      </c>
+      <c r="C20" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>44978</v>
+      </c>
+      <c r="B21" s="8">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -882,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,19 +996,28 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6">
+        <v>44978</v>
+      </c>
+      <c r="B8" s="5">
+        <f>SUM(Journal!C20:C21)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5">
-        <f>SUM(B2:B7)</f>
-        <v>0.79513888888888884</v>
+      <c r="B9" s="5">
+        <f>SUM(B2:B8)</f>
+        <v>0.85763888888888884</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B8 B4" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Création du contrat d'allternance
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Jour</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>Rédaction des problèmes techniques dans le rapport de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analyse du tableau de bord du parc informatique </t>
+  </si>
+  <si>
+    <t>Contrat</t>
+  </si>
+  <si>
+    <t>Rédaction du contrat d'altérnance pour le pré TPI et le TPI</t>
   </si>
 </sst>
 </file>
@@ -250,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E23" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E23"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="7"/>
     <tableColumn id="2" name="Semaine" dataDxfId="6"/>
@@ -264,12 +273,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B9" totalsRowCount="1">
-  <autoFilter ref="A1:B8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B10" totalsRowCount="1">
+  <autoFilter ref="A1:B9"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B8)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B9)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -539,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,6 +920,40 @@
         <v>26</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>44980</v>
+      </c>
+      <c r="B22" s="8">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>44980</v>
+      </c>
+      <c r="B23" s="8">
+        <v>3</v>
+      </c>
+      <c r="C23" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -922,10 +965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,19 +1048,28 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6">
+        <v>44980</v>
+      </c>
+      <c r="B9" s="5">
+        <f>SUM(Journal!C22:C23)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5">
-        <f>SUM(B2:B8)</f>
-        <v>0.85763888888888884</v>
+      <c r="B10" s="5">
+        <f>SUM(B2:B9)</f>
+        <v>0.92013888888888884</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B8 B4" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B9 B4" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Ajout du dossier de conception dans le rapport de projet
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Jour</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Rédaction du contrat d'altérnance pour le pré TPI et le TPI</t>
+  </si>
+  <si>
+    <t>Rédaction du dossier de conception dans le rapport de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction du résumé de projet </t>
   </si>
 </sst>
 </file>
@@ -203,11 +209,11 @@
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
@@ -259,8 +265,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E23" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E25" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:E25"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="7"/>
     <tableColumn id="2" name="Semaine" dataDxfId="6"/>
@@ -276,8 +282,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B10" totalsRowCount="1">
   <autoFilter ref="A1:B9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="1"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="0">
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>SUM(B2:B9)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -548,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,6 +958,38 @@
       </c>
       <c r="E23" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>44981</v>
+      </c>
+      <c r="B24" s="8">
+        <v>3</v>
+      </c>
+      <c r="C24" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>44981</v>
+      </c>
+      <c r="B25" s="8">
+        <v>3</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rédaction du résumé de projet
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Jour</t>
   </si>
@@ -123,15 +123,19 @@
     <t>Rédaction du dossier de conception dans le rapport de projet</t>
   </si>
   <si>
-    <t xml:space="preserve">Rédaction du résumé de projet </t>
+    <t>Création du deuxième et troisième sprint sur Icesrcum</t>
+  </si>
+  <si>
+    <t>Rédaction du résumé du projet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="167" formatCode="[hh]/mm&quot; h&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -169,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,16 +204,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="167" formatCode="[hh]/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
@@ -265,13 +267,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E25" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:E26"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Jour" dataDxfId="7"/>
-    <tableColumn id="2" name="Semaine" dataDxfId="6"/>
-    <tableColumn id="3" name="Temps [h]" dataDxfId="5"/>
-    <tableColumn id="4" name="Type" dataDxfId="4"/>
+    <tableColumn id="1" name="Jour" dataDxfId="6"/>
+    <tableColumn id="2" name="Semaine" dataDxfId="5"/>
+    <tableColumn id="3" name="Temps [h]" dataDxfId="4"/>
+    <tableColumn id="4" name="Type" dataDxfId="3"/>
     <tableColumn id="5" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -279,12 +281,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B10" totalsRowCount="1">
-  <autoFilter ref="A1:B9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B11" totalsRowCount="1">
+  <autoFilter ref="A1:B10"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B9)</totalsRowFormula>
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(B2:B10)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -554,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +567,7 @@
     <col min="1" max="1" width="11.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -984,12 +986,31 @@
       <c r="B25" s="8">
         <v>3</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="D25" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>44981</v>
+      </c>
+      <c r="B26" s="8">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1003,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,19 +1116,28 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="6">
+        <v>44981</v>
+      </c>
+      <c r="B10" s="5">
+        <f>SUM(Journal!C24:C26)</f>
+        <v>0.10069444444444445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5">
-        <f>SUM(B2:B9)</f>
-        <v>0.92013888888888884</v>
+      <c r="B11" s="12">
+        <f>SUM(B2:B10)</f>
+        <v>1.0208333333333333</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B9 B4" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B10 B4" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Création du document pour la gestion des entretiens
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Jour</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>Rédaction du résumé du projet</t>
+  </si>
+  <si>
+    <t>Tests des différents profils sur la nouvelle version version de l'application</t>
+  </si>
+  <si>
+    <t>Rédaction d'une description des analyses faites sur le rapport de projet</t>
+  </si>
+  <si>
+    <t>Fermeture du premier spint</t>
+  </si>
+  <si>
+    <t>Ouverture du deuxième sprint</t>
+  </si>
+  <si>
+    <t>Rédaction des futures questions à poser pour les entretiens</t>
   </si>
 </sst>
 </file>
@@ -135,7 +150,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
-    <numFmt numFmtId="167" formatCode="[hh]/mm&quot; h&quot;;@"/>
+    <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -204,14 +219,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="167" formatCode="[hh]/mm&quot; h&quot;;@"/>
+      <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
@@ -267,8 +282,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:E31"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
@@ -281,12 +296,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B11" totalsRowCount="1">
-  <autoFilter ref="A1:B10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B12" totalsRowCount="1">
+  <autoFilter ref="A1:B11"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B10)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B11)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -556,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,6 +1028,91 @@
         <v>33</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>44984</v>
+      </c>
+      <c r="B27" s="8">
+        <v>4</v>
+      </c>
+      <c r="C27" s="9">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>44984</v>
+      </c>
+      <c r="B28" s="8">
+        <v>4</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>44984</v>
+      </c>
+      <c r="B29" s="8">
+        <v>4</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>44984</v>
+      </c>
+      <c r="B30" s="8">
+        <v>4</v>
+      </c>
+      <c r="C30" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>44984</v>
+      </c>
+      <c r="B31" s="8">
+        <v>4</v>
+      </c>
+      <c r="C31" s="9">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1024,10 +1124,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,11 +1225,16 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6">
+        <v>44984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12">
-        <f>SUM(B2:B10)</f>
+      <c r="B12" s="12">
+        <f>SUM(B2:B11)</f>
         <v>1.0208333333333333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Export des types et des logiciels
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Jour</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>Rédaction des futures questions à poser pour les entretiens</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>J'ai rencontré beaucoup de difficulté à formuler et a trouver des questions pour ce document</t>
+  </si>
+  <si>
+    <t>Export des différents types de composant dans un document Word</t>
+  </si>
+  <si>
+    <t>Export des différents logiciels dans un document Word</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +177,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -188,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,6 +238,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -282,26 +303,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E31" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:E31"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F34" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F34"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
     <tableColumn id="3" name="Temps [h]" dataDxfId="4"/>
     <tableColumn id="4" name="Type" dataDxfId="3"/>
     <tableColumn id="5" name="Description"/>
+    <tableColumn id="6" name="Commentaire"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B12" totalsRowCount="1">
-  <autoFilter ref="A1:B11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B13" totalsRowCount="1">
+  <autoFilter ref="A1:B12"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B11)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B12)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -571,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,9 +606,10 @@
     <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="106.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,8 +625,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>44960</v>
       </c>
@@ -620,7 +646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>44960</v>
       </c>
@@ -637,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>44960</v>
       </c>
@@ -654,7 +680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>44960</v>
       </c>
@@ -671,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>44963</v>
       </c>
@@ -688,7 +714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>44963</v>
       </c>
@@ -705,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>44963</v>
       </c>
@@ -722,7 +748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>44963</v>
       </c>
@@ -739,7 +765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>44964</v>
       </c>
@@ -756,7 +782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>44964</v>
       </c>
@@ -773,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>44966</v>
       </c>
@@ -790,7 +816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>44967</v>
       </c>
@@ -807,7 +833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>44967</v>
       </c>
@@ -824,7 +850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>44967</v>
       </c>
@@ -841,7 +867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>44977</v>
       </c>
@@ -858,7 +884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>44977</v>
       </c>
@@ -875,7 +901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>44977</v>
       </c>
@@ -892,7 +918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>44977</v>
       </c>
@@ -909,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>44978</v>
       </c>
@@ -926,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>44978</v>
       </c>
@@ -943,7 +969,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>44980</v>
       </c>
@@ -960,7 +986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>44980</v>
       </c>
@@ -977,7 +1003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>44981</v>
       </c>
@@ -994,7 +1020,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>44981</v>
       </c>
@@ -1011,7 +1037,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>44981</v>
       </c>
@@ -1028,7 +1054,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>44984</v>
       </c>
@@ -1045,7 +1071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>44984</v>
       </c>
@@ -1053,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="9">
-        <v>3.125E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>6</v>
@@ -1062,7 +1088,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>44984</v>
       </c>
@@ -1079,7 +1105,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>44984</v>
       </c>
@@ -1087,7 +1113,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="9">
-        <v>4.1666666666666664E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>6</v>
@@ -1096,7 +1122,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>44984</v>
       </c>
@@ -1104,13 +1130,67 @@
         <v>4</v>
       </c>
       <c r="C31" s="9">
-        <v>5.5555555555555552E-2</v>
+        <v>5.9027777777777783E-2</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E31" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B32" s="8">
+        <v>4</v>
+      </c>
+      <c r="C32" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B33" s="8">
+        <v>4</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B34" s="8">
+        <v>4</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1124,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,21 +1308,34 @@
       <c r="A11" s="6">
         <v>44984</v>
       </c>
+      <c r="B11" s="5">
+        <f>SUM(Journal!C27:C31)</f>
+        <v>0.21875000000000003</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="6">
+        <v>44985</v>
+      </c>
+      <c r="B12" s="5">
+        <f>SUM(Journal!C32:C34)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="12">
-        <f>SUM(B2:B11)</f>
-        <v>1.0208333333333333</v>
+      <c r="B13" s="12">
+        <f>SUM(B2:B12)</f>
+        <v>1.3020833333333333</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B10 B4" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B11 B4 B12" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Reformulation des questions sur la gestion des entretiens
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t>Jour</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Rédaction des futures questions à poser pour les entretiens</t>
   </si>
   <si>
-    <t>Commentaire</t>
-  </si>
-  <si>
     <t>J'ai rencontré beaucoup de difficulté à formuler et a trouver des questions pour ce document</t>
   </si>
   <si>
@@ -154,6 +151,18 @@
   </si>
   <si>
     <t>Export des différents logiciels dans un document Word</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Séance de review avec les personnes d'Eldora</t>
+  </si>
+  <si>
+    <t>Commentaire/Remarque</t>
+  </si>
+  <si>
+    <t>Reformulation de toutes les questions sur la gestion des entretiens</t>
   </si>
 </sst>
 </file>
@@ -303,27 +312,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F34" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:F34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F38" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F38"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
     <tableColumn id="3" name="Temps [h]" dataDxfId="4"/>
     <tableColumn id="4" name="Type" dataDxfId="3"/>
     <tableColumn id="5" name="Description"/>
-    <tableColumn id="6" name="Commentaire"/>
+    <tableColumn id="6" name="Commentaire/Remarque"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B13" totalsRowCount="1">
-  <autoFilter ref="A1:B12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B15" totalsRowCount="1">
+  <autoFilter ref="A1:B14"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B12)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B14)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -593,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1156,7 +1165,7 @@
         <v>38</v>
       </c>
       <c r="F32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1173,7 +1182,7 @@
         <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1190,7 +1199,75 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>44987</v>
+      </c>
+      <c r="B35" s="8">
+        <v>4</v>
+      </c>
+      <c r="C35" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>44987</v>
+      </c>
+      <c r="B36" s="8">
+        <v>4</v>
+      </c>
+      <c r="C36" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>44988</v>
+      </c>
+      <c r="B37" s="8">
+        <v>4</v>
+      </c>
+      <c r="C37" s="9">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>44988</v>
+      </c>
+      <c r="B38" s="8">
+        <v>4</v>
+      </c>
+      <c r="C38" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1204,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,19 +1400,37 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="6">
+        <v>44987</v>
+      </c>
+      <c r="B13" s="5">
+        <f>SUM(Journal!C35:C36)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>44988</v>
+      </c>
+      <c r="B14" s="5">
+        <f>SUM(Journal!C37:C38)</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="12">
-        <f>SUM(B2:B12)</f>
-        <v>1.3020833333333333</v>
+      <c r="B15" s="12">
+        <f>SUM(B2:B14)</f>
+        <v>1.4583333333333333</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B11 B4 B12" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B14" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Ajout du rapport d entretien Support
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreTPI\PreTPI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\preTPI\PreTPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>Jour</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Organisation des différents entretiens pour le vendredi 10 mars</t>
+  </si>
+  <si>
+    <t>Préparation des documens pour un entretien</t>
+  </si>
+  <si>
+    <t>Entretien avec le responsable du support IT</t>
+  </si>
+  <si>
+    <t>Mettre les demandes/remarques au propre dans un document Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification des exports suite à l'entretien </t>
   </si>
 </sst>
 </file>
@@ -221,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +267,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,8 +333,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F41" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:F41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F47" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F47"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
@@ -333,12 +348,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B15" totalsRowCount="1">
-  <autoFilter ref="A1:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B18" totalsRowCount="1">
+  <autoFilter ref="A1:B17"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B14)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B17)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -608,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,6 +1342,108 @@
         <v>10</v>
       </c>
     </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>44992</v>
+      </c>
+      <c r="B42" s="8">
+        <v>5</v>
+      </c>
+      <c r="C42" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B43" s="14">
+        <v>5</v>
+      </c>
+      <c r="C43" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B44" s="8">
+        <v>5</v>
+      </c>
+      <c r="C44" s="9">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B45" s="8">
+        <v>5</v>
+      </c>
+      <c r="C45" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B46" s="8">
+        <v>5</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B47" s="8">
+        <v>5</v>
+      </c>
+      <c r="C47" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1338,10 +1455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,19 +1592,46 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="6">
+        <v>44991</v>
+      </c>
+      <c r="B15" s="5">
+        <f>SUM(Journal!C39:C41)</f>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>44992</v>
+      </c>
+      <c r="B16" s="5">
+        <f>SUM(Journal!C42)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>44995</v>
+      </c>
+      <c r="B17" s="5">
+        <f>SUM(Journal!C43:C47)</f>
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12">
-        <f>SUM(B2:B14)</f>
-        <v>1.4583333333333333</v>
+      <c r="B18" s="12">
+        <f>SUM(B2:B17)</f>
+        <v>1.8645833333333333</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B14" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B15 B17" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Redaction de 2 rapports d entretien
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
   <si>
     <t>Jour</t>
   </si>
@@ -177,10 +177,22 @@
     <t>Entretien avec le responsable du support IT</t>
   </si>
   <si>
-    <t>Mettre les demandes/remarques au propre dans un document Word</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modification des exports suite à l'entretien </t>
+  </si>
+  <si>
+    <t>Entretien avec le responsable infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rédaction d'un rapport d'entretien </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entretien avec l'équipe de développement </t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Configuration des catégories pour le service Développement</t>
   </si>
 </sst>
 </file>
@@ -333,8 +345,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F47" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:F47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F52" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F52"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
@@ -623,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,7 +1419,7 @@
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,7 +1436,7 @@
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1442,6 +1454,91 @@
       </c>
       <c r="E47" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B48" s="8">
+        <v>5</v>
+      </c>
+      <c r="C48" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B49" s="8">
+        <v>5</v>
+      </c>
+      <c r="C49" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B50" s="8">
+        <v>5</v>
+      </c>
+      <c r="C50" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B51" s="8">
+        <v>5</v>
+      </c>
+      <c r="C51" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>44995</v>
+      </c>
+      <c r="B52" s="8">
+        <v>5</v>
+      </c>
+      <c r="C52" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1458,7 +1555,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,8 +1711,8 @@
         <v>44995</v>
       </c>
       <c r="B17" s="5">
-        <f>SUM(Journal!C43:C47)</f>
-        <v>0.15625</v>
+        <f>SUM(Journal!C43:C52)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1721,7 @@
       </c>
       <c r="B18" s="12">
         <f>SUM(B2:B17)</f>
-        <v>1.8645833333333333</v>
+        <v>2.0416666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de 2 rapports d entretien du 17 mars
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
   <si>
     <t>Jour</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Analyse des templates dans la partie "gestion du parc"</t>
   </si>
   <si>
-    <t>Analyse des fermetures de ticket dans la partie "gestion des tckets"</t>
-  </si>
-  <si>
     <t>Rédaction des problèmes techniques dans le rapport de projet</t>
   </si>
   <si>
@@ -117,27 +114,15 @@
     <t>Contrat</t>
   </si>
   <si>
-    <t>Rédaction du contrat d'altérnance pour le pré TPI et le TPI</t>
-  </si>
-  <si>
     <t>Rédaction du dossier de conception dans le rapport de projet</t>
   </si>
   <si>
-    <t>Création du deuxième et troisième sprint sur Icesrcum</t>
-  </si>
-  <si>
     <t>Rédaction du résumé du projet</t>
   </si>
   <si>
-    <t>Tests des différents profils sur la nouvelle version version de l'application</t>
-  </si>
-  <si>
     <t>Rédaction d'une description des analyses faites sur le rapport de projet</t>
   </si>
   <si>
-    <t>Fermeture du premier spint</t>
-  </si>
-  <si>
     <t>Ouverture du deuxième sprint</t>
   </si>
   <si>
@@ -171,9 +156,6 @@
     <t>Organisation des différents entretiens pour le vendredi 10 mars</t>
   </si>
   <si>
-    <t>Préparation des documens pour un entretien</t>
-  </si>
-  <si>
     <t>Entretien avec le responsable du support IT</t>
   </si>
   <si>
@@ -193,6 +175,54 @@
   </si>
   <si>
     <t>Configuration des catégories pour le service Développement</t>
+  </si>
+  <si>
+    <t>Finalisation de ce qui a été fait le vendredi 10 mars</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Tests des notifications sur la nouvelle version de GLPI</t>
+  </si>
+  <si>
+    <t>Préparation des documents pour un entretien</t>
+  </si>
+  <si>
+    <t>Analyse des fermetures de ticket dans la partie "gestion des tickets"</t>
+  </si>
+  <si>
+    <t>Rédaction du contrat d'alternance pour le pré TPI et le TPI</t>
+  </si>
+  <si>
+    <t>Création du deuxième et troisième sprint sur Icescrum</t>
+  </si>
+  <si>
+    <t>Tests des différents profils sur la nouvelle version  de l'application</t>
+  </si>
+  <si>
+    <t>Fermeture du premier sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration des profils utilisateurs selon les demandes reçus </t>
+  </si>
+  <si>
+    <t>Les profiles Admin, Super-Admin, Technician et Post-Only ont été configuré</t>
+  </si>
+  <si>
+    <t>Entretien avec le responsable sur service de communication digitale</t>
+  </si>
+  <si>
+    <t>Configuration des catégories pour le service Support/Infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entretien avec le responsable du système de gestion </t>
+  </si>
+  <si>
+    <t>Rédacton du rapport de projet</t>
+  </si>
+  <si>
+    <t>Point de situation avec le responsable de projet de chez Eldora</t>
   </si>
 </sst>
 </file>
@@ -345,8 +375,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F52" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:F52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F66" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F66"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
@@ -360,12 +390,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B18" totalsRowCount="1">
-  <autoFilter ref="A1:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B21" totalsRowCount="1">
+  <autoFilter ref="A1:B20"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B17)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B20)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -635,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +677,7 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="75.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="106.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -668,7 +698,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -991,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1008,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1025,7 +1055,7 @@
         <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,10 +1069,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1059,7 +1089,7 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1076,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1093,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1110,7 +1140,7 @@
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1144,7 +1174,7 @@
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1161,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1178,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1195,10 +1225,10 @@
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1215,7 +1245,7 @@
         <v>19</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1232,7 +1262,7 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,10 +1276,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1331,10 +1361,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,10 +1412,10 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,10 +1429,10 @@
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E44" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,7 +1449,7 @@
         <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,7 +1466,7 @@
         <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,13 +1497,13 @@
         <v>3.125E-2</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>44995</v>
       </c>
@@ -1487,10 +1517,10 @@
         <v>6</v>
       </c>
       <c r="E49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>44995</v>
       </c>
@@ -1501,13 +1531,13 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>44995</v>
       </c>
@@ -1521,10 +1551,10 @@
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>44995</v>
       </c>
@@ -1535,11 +1565,242 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>55</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>44998</v>
+      </c>
+      <c r="B53" s="8">
+        <v>6</v>
+      </c>
+      <c r="C53" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>44998</v>
+      </c>
+      <c r="B54" s="8">
+        <v>6</v>
+      </c>
+      <c r="C54" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>44999</v>
+      </c>
+      <c r="B55" s="8">
+        <v>6</v>
+      </c>
+      <c r="C55" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B56" s="8">
+        <v>6</v>
+      </c>
+      <c r="C56" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B57" s="8">
+        <v>6</v>
+      </c>
+      <c r="C57" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E57" t="s">
+        <v>59</v>
+      </c>
+      <c r="F57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B58" s="8">
+        <v>6</v>
+      </c>
+      <c r="C58" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B59" s="8">
+        <v>6</v>
+      </c>
+      <c r="C59" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B60" s="8">
+        <v>6</v>
+      </c>
+      <c r="C60" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B61" s="8">
+        <v>6</v>
+      </c>
+      <c r="C61" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B62" s="8">
+        <v>6</v>
+      </c>
+      <c r="C62" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B63" s="8">
+        <v>6</v>
+      </c>
+      <c r="C63" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B64" s="8">
+        <v>6</v>
+      </c>
+      <c r="C64" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="7">
+        <v>45002</v>
+      </c>
+      <c r="B65" s="8">
+        <v>6</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1552,10 +1813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,19 +1977,46 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="6">
+        <v>44998</v>
+      </c>
+      <c r="B18" s="5">
+        <f>SUM(Journal!C53:C54)</f>
+        <v>0.10416666666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>44999</v>
+      </c>
+      <c r="B19" s="5">
+        <f>SUM(Journal!C55)</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>45002</v>
+      </c>
+      <c r="B20" s="5">
+        <f>SUM(Journal!C56:C64)</f>
+        <v>0.29166666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="12">
-        <f>SUM(B2:B17)</f>
-        <v>2.0416666666666665</v>
+      <c r="B21" s="12">
+        <f>SUM(B2:B20)</f>
+        <v>2.4999999999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B15 B17" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B15 B17:B18 B20" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Deposition de tous les rapports d entretien
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
   <si>
     <t>Jour</t>
   </si>
@@ -223,6 +223,21 @@
   </si>
   <si>
     <t>Point de situation avec le responsable de projet de chez Eldora</t>
+  </si>
+  <si>
+    <t>Entretien avec le responsable du système d'encaissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration des catégories pour le service d'encaissement </t>
+  </si>
+  <si>
+    <t>Configuration de toutes catégories + gabarit de tickets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entretier avec la responsable du service de Qualité &amp; Durabilité </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration de l'annuaire LDAP </t>
   </si>
 </sst>
 </file>
@@ -275,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,6 +326,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -375,8 +393,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F66" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:F66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F75" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:F75"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Jour" dataDxfId="6"/>
     <tableColumn id="2" name="Semaine" dataDxfId="5"/>
@@ -390,12 +408,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B21" totalsRowCount="1">
-  <autoFilter ref="A1:B20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B22" totalsRowCount="1">
+  <autoFilter ref="A1:B21"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(B2:B20)</totalsRowFormula>
+      <totalsRowFormula>SUM(B2:B21)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -665,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,7 +1806,9 @@
       <c r="B65" s="8">
         <v>6</v>
       </c>
-      <c r="C65" s="9"/>
+      <c r="C65" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D65" s="8" t="s">
         <v>41</v>
       </c>
@@ -1797,10 +1817,174 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="8"/>
+      <c r="A66" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B66" s="8">
+        <v>7</v>
+      </c>
+      <c r="C66" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B67" s="8">
+        <v>7</v>
+      </c>
+      <c r="C67" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B68" s="8">
+        <v>7</v>
+      </c>
+      <c r="C68" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B69" s="8">
+        <v>7</v>
+      </c>
+      <c r="C69" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B70" s="8">
+        <v>7</v>
+      </c>
+      <c r="C70" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B71" s="8">
+        <v>7</v>
+      </c>
+      <c r="C71" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B72" s="8">
+        <v>7</v>
+      </c>
+      <c r="C72" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B73" s="8">
+        <v>7</v>
+      </c>
+      <c r="C73" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B74" s="8">
+        <v>7</v>
+      </c>
+      <c r="C74" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>45009</v>
+      </c>
+      <c r="B75" s="8">
+        <v>7</v>
+      </c>
+      <c r="C75" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1813,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1999,24 +2183,33 @@
         <v>45002</v>
       </c>
       <c r="B20" s="5">
-        <f>SUM(Journal!C56:C64)</f>
-        <v>0.29166666666666663</v>
+        <f>SUM(Journal!C56:C65)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="6">
+        <v>45009</v>
+      </c>
+      <c r="B21" s="5">
+        <f>SUM(Journal!C66:C75)</f>
+        <v>0.31249999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="12">
-        <f>SUM(B2:B20)</f>
-        <v>2.4999999999999996</v>
+      <c r="B22" s="12">
+        <f>SUM(B2:B21)</f>
+        <v>2.8541666666666665</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B15 B17:B18 B20" formulaRange="1"/>
+    <ignoredError sqref="B2:B3 B6:B11 B4 B12:B15 B17:B18 B20:B21" formulaRange="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Rendu final du preTPI
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\preTPI\PreTPI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreTPI\PreTPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
   <si>
     <t>Jour</t>
   </si>
@@ -219,9 +219,6 @@
     <t xml:space="preserve">Entretien avec le responsable du système de gestion </t>
   </si>
   <si>
-    <t>Rédacton du rapport de projet</t>
-  </si>
-  <si>
     <t>Point de situation avec le responsable de projet de chez Eldora</t>
   </si>
   <si>
@@ -234,10 +231,10 @@
     <t>Configuration de toutes catégories + gabarit de tickets</t>
   </si>
   <si>
-    <t xml:space="preserve">Entretier avec la responsable du service de Qualité &amp; Durabilité </t>
-  </si>
-  <si>
     <t xml:space="preserve">Configuration de l'annuaire LDAP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entretien avec la responsable du service de Qualité &amp; Durabilité </t>
   </si>
 </sst>
 </file>
@@ -685,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,7 +1793,7 @@
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1813,7 +1810,7 @@
         <v>41</v>
       </c>
       <c r="E65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,7 +1844,7 @@
         <v>41</v>
       </c>
       <c r="E67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1881,7 +1878,7 @@
         <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,7 +1895,7 @@
         <v>48</v>
       </c>
       <c r="E70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1909,7 +1906,7 @@
         <v>7</v>
       </c>
       <c r="C71" s="9">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>6</v>
@@ -1966,7 +1963,7 @@
         <v>48</v>
       </c>
       <c r="E74" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1999,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,7 +2190,7 @@
       </c>
       <c r="B21" s="5">
         <f>SUM(Journal!C66:C75)</f>
-        <v>0.31249999999999994</v>
+        <v>0.33333333333333326</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2202,7 +2199,7 @@
       </c>
       <c r="B22" s="12">
         <f>SUM(B2:B21)</f>
-        <v>2.8541666666666665</v>
+        <v>2.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>